<commit_message>
Received data from Ergast, started on replication job
</commit_message>
<xml_diff>
--- a/F1EncyclopediaSeedData.xlsx
+++ b/F1EncyclopediaSeedData.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7371be6fed90226b/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mikey\source\repos\F1Encyclopedia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="313" documentId="8_{7FB53C6D-F833-4A3C-A46C-0DCB4A1DC893}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{49AB3DFC-77E4-46B5-8C50-2EFFA2E244ED}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6DA5FC-0974-4A38-AF36-3B7218ED12CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="1860" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{F2F025FC-370A-47C5-9CFB-AA450EB719C7}"/>
+    <workbookView xWindow="3780" yWindow="1860" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="6" xr2:uid="{F2F025FC-370A-47C5-9CFB-AA450EB719C7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Countries" sheetId="1" r:id="rId1"/>
-    <sheet name="PersonRoles" sheetId="6" r:id="rId2"/>
-    <sheet name="RaceWeekends" sheetId="7" r:id="rId3"/>
-    <sheet name="Tracks" sheetId="8" r:id="rId4"/>
+    <sheet name="PersonRoles" sheetId="6" r:id="rId1"/>
+    <sheet name="RaceWeekends" sheetId="7" r:id="rId2"/>
+    <sheet name="Tracks" sheetId="8" r:id="rId3"/>
+    <sheet name="Countries" sheetId="1" r:id="rId4"/>
     <sheet name="Colours" sheetId="3" r:id="rId5"/>
     <sheet name="Persons" sheetId="2" r:id="rId6"/>
     <sheet name="Constructors" sheetId="5" r:id="rId7"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="114">
   <si>
     <t>Name</t>
   </si>
@@ -376,6 +376,12 @@
   </si>
   <si>
     <t>Country</t>
+  </si>
+  <si>
+    <t>Laps</t>
+  </si>
+  <si>
+    <t>WinnerId</t>
   </si>
 </sst>
 </file>
@@ -728,6 +734,96 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19F87DC-BC4C-4D76-8060-3502C783844E}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4127493-794A-4896-BBE7-8070008EA6AC}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{466719E4-643C-484F-97E5-C0EADB392D1E}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B76B35-AEE1-4662-8EA5-5FF9831B4F8C}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -858,87 +954,6 @@
       </c>
       <c r="B15" t="s">
         <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19F87DC-BC4C-4D76-8060-3502C783844E}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4127493-794A-4896-BBE7-8070008EA6AC}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{466719E4-643C-484F-97E5-C0EADB392D1E}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1516,7 +1531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A79E4F1F-9711-4DAE-9154-FEC1421FDDB8}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>